<commit_message>
SURVEY REGRESSION NOT FINISHED
</commit_message>
<xml_diff>
--- a/data/survey_data/final.xlsx
+++ b/data/survey_data/final.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -42,13 +42,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -106,27 +112,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -440,1344 +449,1334 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>19</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>1001</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>40</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>32</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>29</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>28</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>1002</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="6">
         <v>40</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="6">
         <v>24</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <v>24</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>33</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="6">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>21</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>1003</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="6">
         <v>27</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>37</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>32</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>21</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="4">
+      <c r="A5" s="5">
         <v>45</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>1004</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="6">
         <v>32</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>45</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>35</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>25</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <v>10</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="6">
         <v>1005</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="6">
         <v>32</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>40</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>38</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="6">
         <v>20</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="4">
+      <c r="A7" s="5">
         <v>31</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <v>1006</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <v>21</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>52</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>43</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <v>18</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="6">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="4">
+      <c r="A8" s="5">
         <v>9</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="6">
         <v>1007</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="6">
         <v>21</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>46</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>38</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="6">
         <v>17</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="4">
+      <c r="A9" s="5">
         <v>17</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="6">
         <v>1008</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="6">
         <v>40</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>25</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>26</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="6">
         <v>32</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="6">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="4">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+      <c r="A10" s="5">
         <v>13</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="6">
         <v>1009</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="6">
         <v>21</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>48</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <v>44</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="6">
         <v>9</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="6">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="4">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
+      <c r="A11" s="5">
         <v>18</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
         <v>1010</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="6">
         <v>28</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>47</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>39</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="6">
         <v>19</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="6">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="4">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
+      <c r="A12" s="5">
         <v>14</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="6">
         <v>1011</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="6">
         <v>34</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>39</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <v>39</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="6">
         <v>23</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="6">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="4">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="6">
         <v>1012</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="6">
         <v>35</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>37</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="6">
         <v>38</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="6">
         <v>25</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="6">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="4">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+      <c r="A14" s="5">
         <v>1</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>1013</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>29</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>45</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <v>43</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="6">
         <v>20</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="6">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="4">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+      <c r="A15" s="5">
         <v>15</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>1015</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>31</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>47</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <v>53</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="6">
         <v>26</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="6">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="4">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+      <c r="A16" s="5">
         <v>20</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="6">
         <v>1016</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="6">
         <v>35</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>31</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>25</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="6">
         <v>28</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="4">
+      <c r="A17" s="5">
         <v>27</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>1017</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>38</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>40</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="6">
         <v>29</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6">
         <v>24</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="6">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="4">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>1018</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>30</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>37</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>35</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>23</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="6">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="4">
+      <c r="A19" s="5">
         <v>26</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>1019</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>31</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>33</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>34</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
         <v>22</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="6">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="4">
+      <c r="A20" s="5">
         <v>7</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>1020</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="6">
         <v>30</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>47</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="6">
         <v>48</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="6">
         <v>23</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="4">
+      <c r="A21" s="5">
         <v>3</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>1021</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="6">
         <v>40</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>30</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="6">
         <v>27</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="6">
         <v>15</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="15.75">
-      <c r="A22" s="4">
+      <c r="A22" s="5">
         <v>4</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>1022</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>21</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>49</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="6">
         <v>41</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="6">
         <v>17</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
-      <c r="A23" s="4">
+      <c r="A23" s="5">
         <v>0</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>1023</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>21</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>47</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="6">
         <v>36</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>9</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="15.75">
-      <c r="A24" s="4">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>1025</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <v>39</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>28</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="6">
         <v>26</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="6">
         <v>23</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="15.75">
-      <c r="A25" s="4">
+      <c r="A25" s="5">
         <v>55</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>1026</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>34</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>35</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="6">
         <v>36</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>19</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="15.75">
-      <c r="A26" s="4">
+      <c r="A26" s="5">
         <v>2</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>1027</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="6">
         <v>30</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>34</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="6">
         <v>26</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="6">
         <v>23</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="15.75">
-      <c r="A27" s="4">
+      <c r="A27" s="5">
         <v>22</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>1028</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="6">
         <v>37</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="6">
         <v>40</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="6">
         <v>27</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="6">
         <v>29</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="15.75">
-      <c r="A28" s="4">
+      <c r="A28" s="5">
         <v>54</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>1029</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="6">
         <v>31</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>40</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="6">
         <v>43</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="6">
         <v>22</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="15.75">
-      <c r="A29" s="4">
+      <c r="A29" s="5">
         <v>25</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>1030</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="6">
         <v>32</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>39</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="6">
         <v>31</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="6">
         <v>23</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="15.75">
-      <c r="A30" s="4">
+      <c r="A30" s="5">
         <v>5</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>1031</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="6">
         <v>31</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="6">
         <v>44</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="6">
         <v>48</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="6">
         <v>17</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="6">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="15.75">
-      <c r="A31" s="4">
+      <c r="A31" s="5">
         <v>24</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>1033</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="6">
         <v>37</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="6">
         <v>34</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="6">
         <v>27</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="6">
         <v>18</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="6">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="15.75">
-      <c r="A32" s="4">
+      <c r="A32" s="5">
         <v>6</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>1034</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="6">
         <v>39</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="6">
         <v>26</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="6">
         <v>31</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="6">
         <v>28</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="15.75">
-      <c r="A33" s="4">
+      <c r="A33" s="5">
         <v>28</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>1035</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="6">
         <v>38</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="6">
         <v>34</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="6">
         <v>28</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="6">
         <v>26</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
-      <c r="A34" s="4">
+      <c r="A34" s="5">
         <v>42</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="6">
         <v>2001</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="6">
         <v>37</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="6">
         <v>34</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="6">
         <v>25</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="6">
         <v>31</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15.75">
-      <c r="A35" s="4">
+      <c r="A35" s="5">
         <v>43</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="6">
         <v>2002</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="6">
         <v>15</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="6">
         <v>46</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="6">
         <v>40</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="6">
         <v>16</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="6">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15.75">
-      <c r="A36" s="4">
+      <c r="A36" s="5">
         <v>51</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="6">
         <v>2003</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="6">
         <v>33</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="6">
         <v>29</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="6">
         <v>25</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="6">
         <v>25</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15.75">
-      <c r="A37" s="4">
+      <c r="A37" s="5">
         <v>29</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="6">
         <v>2004</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="6">
         <v>34</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="6">
         <v>38</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="6">
         <v>28</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="6">
         <v>20</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="15.75">
-      <c r="A38" s="4">
+      <c r="A38" s="5">
         <v>44</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="6">
         <v>2005</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="6">
         <v>40</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="6">
         <v>29</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="6">
         <v>26</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="6">
         <v>27</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="15.75">
-      <c r="A39" s="4">
+      <c r="A39" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="6">
         <v>2006</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="6">
         <v>31</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="6">
         <v>36</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="6">
         <v>26</v>
       </c>
-      <c r="F39" s="5">
+      <c r="F39" s="6">
         <v>27</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15.75">
-      <c r="A40" s="4">
+      <c r="A40" s="5">
         <v>35</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="6">
         <v>2008</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="6">
         <v>21</v>
       </c>
-      <c r="D40" s="5">
+      <c r="D40" s="6">
         <v>48</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="6">
         <v>39</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="6">
         <v>19</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="6">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="15.75">
-      <c r="A41" s="4">
+      <c r="A41" s="5">
         <v>33</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="6">
         <v>2009</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="6">
         <v>25</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="6">
         <v>46</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="6">
         <v>45</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="6">
         <v>16</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="15.75">
-      <c r="A42" s="4">
+      <c r="A42" s="5">
         <v>39</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="6">
         <v>2010</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="6">
         <v>29</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="6">
         <v>37</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="6">
         <v>30</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="6">
         <v>23</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="15.75">
-      <c r="A43" s="4">
+      <c r="A43" s="5">
         <v>32</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>2011</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="6">
         <v>26</v>
       </c>
-      <c r="D43" s="5">
+      <c r="D43" s="6">
         <v>33</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="6">
         <v>27</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F43" s="6">
         <v>23</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="6">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="15.75">
-      <c r="A44" s="4">
+      <c r="A44" s="5">
         <v>36</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="6">
         <v>2012</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="6">
         <v>31</v>
       </c>
-      <c r="D44" s="5">
+      <c r="D44" s="6">
         <v>42</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="6">
         <v>34</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F44" s="6">
         <v>20</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="6">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="15.75">
-      <c r="A45" s="4">
+      <c r="A45" s="5">
         <v>52</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="6">
         <v>2013</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="6">
         <v>37</v>
       </c>
-      <c r="D45" s="5">
+      <c r="D45" s="6">
         <v>30</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="6">
         <v>29</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="6">
         <v>32</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="6">
         <v>2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="15.75">
-      <c r="A46" s="4">
+      <c r="A46" s="5">
         <v>48</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="6">
         <v>2014</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="6">
         <v>39</v>
       </c>
-      <c r="D46" s="5">
+      <c r="D46" s="6">
         <v>33</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="6">
         <v>28</v>
       </c>
-      <c r="F46" s="5">
+      <c r="F46" s="6">
         <v>18</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="15.75">
-      <c r="A47" s="4">
+      <c r="A47" s="5">
         <v>50</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <v>2015</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="6">
         <v>30</v>
       </c>
-      <c r="D47" s="5">
+      <c r="D47" s="6">
         <v>41</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="6">
         <v>37</v>
       </c>
-      <c r="F47" s="5">
+      <c r="F47" s="6">
         <v>22</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="15.75">
-      <c r="A48" s="4">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <v>2016</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="6">
         <v>32</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="6">
         <v>30</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="6">
         <v>25</v>
       </c>
-      <c r="F48" s="5">
+      <c r="F48" s="6">
         <v>16</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="15.75">
-      <c r="A49" s="4">
+      <c r="A49" s="5">
         <v>46</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="6">
         <v>2017</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="6">
         <v>29</v>
       </c>
-      <c r="D49" s="5">
+      <c r="D49" s="6">
         <v>44</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="6">
         <v>45</v>
       </c>
-      <c r="F49" s="5">
+      <c r="F49" s="6">
         <v>15</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="6">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="15.75">
-      <c r="A50" s="4">
+      <c r="A50" s="5">
         <v>40</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="6">
         <v>2018</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="6">
         <v>35</v>
       </c>
-      <c r="D50" s="5">
+      <c r="D50" s="6">
         <v>48</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="6">
         <v>37</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F50" s="6">
         <v>18</v>
       </c>
-      <c r="G50" s="5">
+      <c r="G50" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="15.75">
-      <c r="A51" s="4">
+      <c r="A51" s="5">
         <v>12</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="6">
         <v>2019</v>
       </c>
-      <c r="C51" s="5">
+      <c r="C51" s="6">
         <v>30</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D51" s="6">
         <v>33</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="6">
         <v>31</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F51" s="6">
         <v>11</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="6">
         <v>4</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="15.75">
-      <c r="A52" s="4">
+      <c r="A52" s="5">
         <v>34</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="6">
         <v>2020</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="6">
         <v>27</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="6">
         <v>30</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="6">
         <v>22</v>
       </c>
-      <c r="F52" s="5">
+      <c r="F52" s="6">
         <v>34</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="15.75">
-      <c r="A53" s="4">
+      <c r="A53" s="5">
         <v>38</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="6">
         <v>2021</v>
       </c>
-      <c r="C53" s="5">
+      <c r="C53" s="6">
         <v>39</v>
       </c>
-      <c r="D53" s="5">
+      <c r="D53" s="6">
         <v>22</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="6">
         <v>27</v>
       </c>
-      <c r="F53" s="5">
+      <c r="F53" s="6">
         <v>21</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="15.75">
-      <c r="A54" s="4">
+      <c r="A54" s="5">
         <v>49</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="6">
         <v>2022</v>
       </c>
-      <c r="C54" s="5">
+      <c r="C54" s="6">
         <v>31</v>
       </c>
-      <c r="D54" s="5">
+      <c r="D54" s="6">
         <v>42</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="6">
         <v>42</v>
       </c>
-      <c r="F54" s="5">
+      <c r="F54" s="6">
         <v>27</v>
       </c>
-      <c r="G54" s="5">
+      <c r="G54" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="15.75">
-      <c r="A55" s="4">
+      <c r="A55" s="5">
         <v>53</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="6">
         <v>2023</v>
       </c>
-      <c r="C55" s="5">
+      <c r="C55" s="6">
         <v>39</v>
       </c>
-      <c r="D55" s="5">
+      <c r="D55" s="6">
         <v>34</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="6">
         <v>26</v>
       </c>
-      <c r="F55" s="5">
+      <c r="F55" s="6">
         <v>24</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="15.75">
-      <c r="A56" s="4">
+      <c r="A56" s="5">
         <v>30</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56" s="6">
         <v>2025</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C56" s="6">
         <v>35</v>
       </c>
-      <c r="D56" s="5">
+      <c r="D56" s="6">
         <v>32</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="6">
         <v>26</v>
       </c>
-      <c r="F56" s="5">
+      <c r="F56" s="6">
         <v>24</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="6">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="15.75">
-      <c r="A57" s="4">
+      <c r="A57" s="5">
         <v>41</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="6">
         <v>2026</v>
       </c>
-      <c r="C57" s="5">
+      <c r="C57" s="6">
         <v>24</v>
       </c>
-      <c r="D57" s="5">
+      <c r="D57" s="6">
         <v>46</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="6">
         <v>42</v>
       </c>
-      <c r="F57" s="5">
+      <c r="F57" s="6">
         <v>13</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="6">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="15.75">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7" t="s">
+      <c r="A58" s="7"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="G58" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="15.75">
       <c r="A59" s="1"/>

</xml_diff>